<commit_message>
Add First Hot Metal Bridge, update data
</commit_message>
<xml_diff>
--- a/module-06/lab-06/final-project/EvolutionOfPittsburghBridges/PittsburghBridges.xlsx
+++ b/module-06/lab-06/final-project/EvolutionOfPittsburghBridges/PittsburghBridges.xlsx
@@ -10,14 +10,14 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$K$133</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$K$134</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="270">
   <si>
     <t>Page_Number</t>
   </si>
@@ -406,9 +406,6 @@
     <t>Wooden</t>
   </si>
   <si>
-    <t>Lattice Girder</t>
-  </si>
-  <si>
     <t>Aqueduct</t>
   </si>
   <si>
@@ -422,9 +419,6 @@
   </si>
   <si>
     <t>Beam</t>
-  </si>
-  <si>
-    <t>Monongahela Connecting Railroad Bridge (Hot Metal Street Bridge)</t>
   </si>
   <si>
     <t>Photo_Path</t>
@@ -519,9 +513,6 @@
     <t>Pittsburgh's first bridge over the Allegheny River, an 1819 covered bridge, was replaced by John Roebling’s 1859 suspension bridge (pictured). The bridge company’s director felt that an attractive Roebling bridge would increase revenue. He was right.</t>
   </si>
   <si>
-    <t>By the 1890s, Roebling’s bridge was unable to carry the heavier electric trolleys. The replacement bridge by Theodore Cooper was built around Roebling’s bridge. Construction took 95 days. The bridge was dismantled in 1927 onto barges, floated along the river to be reused at another location.</t>
-  </si>
-  <si>
     <t>By the 1880s, Pittsburgh and Allegheny City (now North Side) had grown to the point that investors felt there would be enough traffic for a crossing at Seventh Street. Gustav Lindenthal, who was working on the 1883 Smithfield Street Bridge, designed the suspension bridge.</t>
   </si>
   <si>
@@ -540,9 +531,6 @@
     <t>Allegheny Aqueduct</t>
   </si>
   <si>
-    <t>Pittsburgh leaders campaigned in the state legislature to build a canal to Philadelphia. The first wooden aqueduct was built in 1829. Its replacement by John Roebling (pictured) was built in 1845, launching his renowned bridge-engineering career.</t>
-  </si>
-  <si>
     <t>First envisioned in the 1930s, Crosstown Boulevard (I-579) was designed and constructed in the 1950s and 1960s to connect the Liberty Bridge to the planned East Street Valley Expressway. The bridge opened in 1989. It is Pittsburgh’s only major steel girder river crossing.</t>
   </si>
   <si>
@@ -660,48 +648,6 @@
     <t>Photos/Allegheny/Highland_Park.jpg</t>
   </si>
   <si>
-    <t>Photos/Allegheny/Wabash.jpg</t>
-  </si>
-  <si>
-    <t>Photos/Allegheny/Smithfield_Street.jpg</t>
-  </si>
-  <si>
-    <t>Photos/Allegheny/First_Panhandle.jpg</t>
-  </si>
-  <si>
-    <t>Photos/Allegheny/Panhandle.jpg</t>
-  </si>
-  <si>
-    <t>Photos/Allegheny/Liberty.jpg</t>
-  </si>
-  <si>
-    <t>Photos/Allegheny/Second_Tenth_Street.jpg</t>
-  </si>
-  <si>
-    <t>Photos/Allegheny/Brady_Street.jpg</t>
-  </si>
-  <si>
-    <t>Photos/Allegheny/Birmingham.jpg</t>
-  </si>
-  <si>
-    <t>Photos/Allegheny/Hot_Metal.jpg</t>
-  </si>
-  <si>
-    <t>Photos/Allegheny/First_Glenwood.jpg</t>
-  </si>
-  <si>
-    <t>Photos/Allegheny/Glenwood.jpg</t>
-  </si>
-  <si>
-    <t>Photos/Allegheny/B_O_Railroad.jpg</t>
-  </si>
-  <si>
-    <t>Photos/Allegheny/Browns.jpg</t>
-  </si>
-  <si>
-    <t>Photos/Allegheny/Homestead_Grays.jpg</t>
-  </si>
-  <si>
     <t>Photos/Ohio/West_End.jpg</t>
   </si>
   <si>
@@ -717,9 +663,6 @@
     <t xml:space="preserve">The Ohio &amp; Pennsylvania Railroad, chartered in 1848, was connected to Pittsburgh in 1857 via a wooden bridge over the Allegheny River. </t>
   </si>
   <si>
-    <t>Pittsburgh leaders campaigned in the state legislature to build a canal to Philadelphia. The first wooden aqueduct was built in 1829.</t>
-  </si>
-  <si>
     <t>An 1856 wooden covered bridge was replaced by the higher Sharpsburg Bridge in 1899-1900.</t>
   </si>
   <si>
@@ -774,43 +717,118 @@
     <t>Photos/Allegheny/Second_Sharpsburg.jpg</t>
   </si>
   <si>
-    <t>Photos/Allegheny/First_Monongahela_Covered.jpg</t>
-  </si>
-  <si>
-    <t>Photos/Allegheny/Second_Monongahela.jpg</t>
-  </si>
-  <si>
     <t>Panhandle Railroad Bridge</t>
   </si>
   <si>
-    <t>Photos/Allegheny/First_Tenth_Street.jpg</t>
-  </si>
-  <si>
     <t>Tenth Street Bridge</t>
   </si>
   <si>
-    <t>Photos/Allegheny/Tenth_Street.jpg</t>
-  </si>
-  <si>
     <t>Glenwood Bridge</t>
   </si>
   <si>
-    <t>Photos/Allegheny/First_B_O_Railroad.jpg</t>
-  </si>
-  <si>
     <t>A Monongahela River crossing was constructed for the Wheeling Branch of the Baltimore &amp; Ohio Railroad between Hays and Glenwood in 1884 to connect its main line in Washington, Pennsylvania, with its Glenwood Yard and its line along the river. Here, the original Whipple truss is being replaced by the current Pennsylvania-truss bridge in 1915.</t>
   </si>
   <si>
     <t>A Monongahela River crossing was constructed for the Wheeling Branch of the Baltimore &amp; Ohio Railroad between Hays and Glenwood in 1884. The original Whipple truss was replaced by the current Pennsylvania truss bridge (pictured) in 1915. The American Bridge Company constructed the new crossing.</t>
   </si>
   <si>
-    <t>The steelmaking process was streamlined when a hot-metal bridge was constructed in 1887 to carry molten iron between factories across the river.</t>
-  </si>
-  <si>
-    <t>The 1887 bridge was replaced in 1901 and widened with an upstream bridge in 1904. The bridges now carry vehicular, pedestrian, and bicycle traffic.</t>
-  </si>
-  <si>
     <t>River_Name</t>
+  </si>
+  <si>
+    <t>Metal Thru Truss</t>
+  </si>
+  <si>
+    <t>Wooden Covered Truss</t>
+  </si>
+  <si>
+    <t>Metal Deck Truss</t>
+  </si>
+  <si>
+    <t>Metal Lattice Girder</t>
+  </si>
+  <si>
+    <t>By the 1890s, Roebling’s bridge was unable to carry the heavier electric trolleys. The replacement bridge by Theodore Cooper was built around Roebling’s bridge. Construction took 95 days. The bridge was dismantled in 1927 onto barges, floated along the river to be reused over the Ohio River to connect Coraopolis and Neville Island. The bridge lasted there until 1994.</t>
+  </si>
+  <si>
+    <t>Early westward transportation routes bypassed Pittsburgh—the 1818 National Road was south, and the 1825 Erie Canal was north. Pittsburgh leaders campaigned in the state legislature to build a canal to Philadelphia. Routes along the Allegheny River were surveyed. The north bank was deemed most suitable, necessitating a wooden aqueduct across the Allegheny River to Pittsburgh at Eleventh Street, built in 1829.</t>
+  </si>
+  <si>
+    <t>Canal engineer John Roebling pioneered the technique of twisting strands of wire into rope. He designed a low-cost replacement bridge for the maintenance-intensive Allegheny Aqueduct using wire rope, and he successfully lobbied the canal company to build the bridge. He invented a mechanized process to band wire ropes together into cables to improve rigidity. Roebling’s 1845 aqueduct was an immediate success, launching his renowned bridge-engineering career.</t>
+  </si>
+  <si>
+    <t>Photos/Monongahela/Second_Monongahela.jpg</t>
+  </si>
+  <si>
+    <t>Photos/Monongahela/Hot_Metal.jpg</t>
+  </si>
+  <si>
+    <t>Photos/Monongahela/First_Monongahela_Covered.jpg</t>
+  </si>
+  <si>
+    <t>Monongahela Connecting Railroad Bridge</t>
+  </si>
+  <si>
+    <t>Iron was smelted at Eliza Furnaces, cast into pig, ferried across the Monongahela River, and reheated for production at Jones and Laughlin’s American Iron Works. The process was streamlined when a hot-metal bridge was constructed in 1887 to carry molten iron directly across the river. Its superstructure was replaced in 1901 and was widened with an upstream bridge in 1904.</t>
+  </si>
+  <si>
+    <t>The 1901 Hot Metal Bridge (left) originally had a fireproof brick deck, replaced by steel plate in 1960 to lighten the bridge for heavier railcars. It was converted to pedestrian and bicycle use in 2007.</t>
+  </si>
+  <si>
+    <t>The 1904 Monongahela Connecting Railroad Bridge (right) carried intra-mill shipments and exports until it was closed in 1993 and converted to vehicular use in 2000.</t>
+  </si>
+  <si>
+    <t>Hot Metal Bridge</t>
+  </si>
+  <si>
+    <t>Photos/Monongahela/First_Hot_Metal.jpg</t>
+  </si>
+  <si>
+    <t>Photos/Monongahela/Wabash.jpg</t>
+  </si>
+  <si>
+    <t>Photos/Monongahela/Smithfield_Street.jpg</t>
+  </si>
+  <si>
+    <t>Photos/Monongahela/First_Panhandle.jpg</t>
+  </si>
+  <si>
+    <t>Photos/Monongahela/Panhandle.jpg</t>
+  </si>
+  <si>
+    <t>Photos/Monongahela/Liberty.jpg</t>
+  </si>
+  <si>
+    <t>Photos/Monongahela/First_Tenth_Street.jpg</t>
+  </si>
+  <si>
+    <t>Photos/Monongahela/Second_Tenth_Street.jpg</t>
+  </si>
+  <si>
+    <t>Photos/Monongahela/Tenth_Street.jpg</t>
+  </si>
+  <si>
+    <t>Photos/Monongahela/Brady_Street.jpg</t>
+  </si>
+  <si>
+    <t>Photos/Monongahela/Birmingham.jpg</t>
+  </si>
+  <si>
+    <t>Photos/Monongahela/First_Glenwood.jpg</t>
+  </si>
+  <si>
+    <t>Photos/Monongahela/Glenwood.jpg</t>
+  </si>
+  <si>
+    <t>Photos/Monongahela/First_B_O_Railroad.jpg</t>
+  </si>
+  <si>
+    <t>Photos/Monongahela/B_O_Railroad.jpg</t>
+  </si>
+  <si>
+    <t>Photos/Monongahela/Browns.jpg</t>
+  </si>
+  <si>
+    <t>Photos/Monongahela/Homestead_Grays.jpg</t>
   </si>
 </sst>
 </file>
@@ -1150,18 +1168,18 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:K133"/>
+  <dimension ref="A1:K134"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
+      <selection pane="bottomLeft" activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="46.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" style="2" bestFit="1" customWidth="1"/>
@@ -1180,7 +1198,7 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>123</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -1199,24 +1217,24 @@
         <v>4</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>263</v>
+        <v>237</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="45">
+    <row r="2" spans="1:11" ht="45" customHeight="1">
       <c r="A2" s="2">
         <v>14</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>127</v>
+      <c r="C2" s="1" t="s">
+        <v>239</v>
       </c>
       <c r="D2" s="2">
         <v>1875</v>
@@ -1237,13 +1255,13 @@
         <v>90</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="60" hidden="1">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="60" customHeight="1">
       <c r="A3" s="2">
         <v>15</v>
       </c>
@@ -1272,10 +1290,10 @@
         <v>107</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="60">
@@ -1285,8 +1303,8 @@
       <c r="B4" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>133</v>
+      <c r="C4" s="1" t="s">
+        <v>238</v>
       </c>
       <c r="D4" s="2">
         <v>1915</v>
@@ -1307,13 +1325,13 @@
         <v>90</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="45" hidden="1">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="45" customHeight="1">
       <c r="A5" s="2">
         <v>18</v>
       </c>
@@ -1321,7 +1339,7 @@
         <v>64</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D5" s="2">
         <v>1927</v>
@@ -1342,19 +1360,20 @@
         <v>107</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" hidden="1">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="15" hidden="1" customHeight="1">
       <c r="A6" s="2">
         <v>20</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>108</v>
       </c>
+      <c r="C6" s="2"/>
       <c r="D6" s="2">
         <v>1963</v>
       </c>
@@ -1370,7 +1389,7 @@
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
     </row>
-    <row r="7" spans="1:11" ht="60" hidden="1">
+    <row r="7" spans="1:11" ht="60" customHeight="1">
       <c r="A7" s="2">
         <v>21</v>
       </c>
@@ -1396,13 +1415,13 @@
         <v>107</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="60">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="60" customHeight="1">
       <c r="A8" s="2">
         <v>23</v>
       </c>
@@ -1428,19 +1447,20 @@
         <v>90</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" hidden="1">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="15" hidden="1" customHeight="1">
       <c r="A9" s="2">
         <v>24</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="C9" s="2"/>
       <c r="F9" s="2">
         <v>40.441896999999997</v>
       </c>
@@ -1453,15 +1473,15 @@
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
     </row>
-    <row r="10" spans="1:11" ht="30">
+    <row r="10" spans="1:11" ht="45" customHeight="1">
       <c r="A10" s="2">
         <v>26</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>127</v>
+      <c r="C10" s="1" t="s">
+        <v>239</v>
       </c>
       <c r="D10" s="2">
         <v>1819</v>
@@ -1482,13 +1502,13 @@
         <v>90</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>237</v>
+        <v>218</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="45">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="45" customHeight="1">
       <c r="A11" s="2">
         <v>26</v>
       </c>
@@ -1517,21 +1537,21 @@
         <v>90</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>238</v>
+        <v>219</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="45">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="60">
       <c r="A12" s="2">
         <v>26</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>133</v>
+      <c r="C12" s="1" t="s">
+        <v>238</v>
       </c>
       <c r="D12" s="2">
         <v>1892</v>
@@ -1552,24 +1572,24 @@
         <v>90</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>239</v>
+        <v>220</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="45">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="45" customHeight="1">
       <c r="A13" s="2">
         <v>28</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>243</v>
+        <v>224</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>124</v>
       </c>
       <c r="D13" s="2">
-        <v>1885</v>
+        <v>1884</v>
       </c>
       <c r="E13" s="2">
         <v>1925</v>
@@ -1587,21 +1607,21 @@
         <v>90</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>240</v>
+        <v>221</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="30">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="45" customHeight="1">
       <c r="A14" s="2">
         <v>29</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>127</v>
+      <c r="C14" s="1" t="s">
+        <v>239</v>
       </c>
       <c r="D14" s="2">
         <v>1839</v>
@@ -1622,10 +1642,10 @@
         <v>90</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>242</v>
+        <v>223</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="60">
@@ -1635,11 +1655,11 @@
       <c r="B15" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>133</v>
+      <c r="C15" s="1" t="s">
+        <v>238</v>
       </c>
       <c r="D15" s="2">
-        <v>1889</v>
+        <v>1890</v>
       </c>
       <c r="E15" s="2">
         <v>1925</v>
@@ -1657,18 +1677,18 @@
         <v>90</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>241</v>
+        <v>222</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="180">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="180" customHeight="1">
       <c r="A16" s="2">
         <v>32</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>244</v>
+        <v>225</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>124</v>
@@ -1689,18 +1709,18 @@
         <v>90</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" ht="180">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="180" customHeight="1">
       <c r="A17" s="2">
         <v>33</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>245</v>
+        <v>226</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>124</v>
@@ -1721,18 +1741,18 @@
         <v>90</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" ht="180">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="180" customHeight="1">
       <c r="A18" s="2">
         <v>33</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>246</v>
+        <v>227</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>124</v>
@@ -1753,13 +1773,13 @@
         <v>90</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" ht="30">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="30" customHeight="1">
       <c r="A19" s="2">
         <v>34</v>
       </c>
@@ -1788,18 +1808,18 @@
         <v>90</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" ht="45">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="45" customHeight="1">
       <c r="A20" s="2">
         <v>34</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C20" s="2" t="s">
-        <v>129</v>
+      <c r="C20" s="1" t="s">
+        <v>241</v>
       </c>
       <c r="D20" s="2">
         <v>1864</v>
@@ -1820,10 +1840,10 @@
         <v>90</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="45">
@@ -1833,8 +1853,8 @@
       <c r="B21" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>133</v>
+      <c r="C21" s="1" t="s">
+        <v>238</v>
       </c>
       <c r="D21" s="2">
         <v>1904</v>
@@ -1852,21 +1872,21 @@
         <v>90</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" ht="30">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="60">
       <c r="A22" s="2">
         <v>36</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D22" s="2">
         <v>1829</v>
@@ -1887,24 +1907,24 @@
         <v>90</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" ht="45">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="75">
       <c r="A23" s="2">
         <v>36</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D23" s="2">
         <v>1845</v>
       </c>
       <c r="E23" s="2">
-        <v>1857</v>
+        <v>1861</v>
       </c>
       <c r="F23" s="2">
         <v>40.448578000000097</v>
@@ -1919,13 +1939,13 @@
         <v>90</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" ht="45">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="45" customHeight="1">
       <c r="A24" s="2">
         <v>37</v>
       </c>
@@ -1933,7 +1953,7 @@
         <v>77</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D24" s="2">
         <v>1989</v>
@@ -1951,21 +1971,21 @@
         <v>90</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" ht="60">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="60" customHeight="1">
       <c r="A25" s="2">
         <v>37</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C25" s="2" t="s">
-        <v>127</v>
+      <c r="C25" s="1" t="s">
+        <v>239</v>
       </c>
       <c r="D25" s="2">
         <v>1837</v>
@@ -1986,13 +2006,13 @@
         <v>90</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" ht="45">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="45" customHeight="1">
       <c r="A26" s="2">
         <v>37</v>
       </c>
@@ -2018,10 +2038,10 @@
         <v>90</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="60">
@@ -2031,8 +2051,8 @@
       <c r="B27" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C27" s="2" t="s">
-        <v>133</v>
+      <c r="C27" s="1" t="s">
+        <v>238</v>
       </c>
       <c r="D27" s="2">
         <v>1903</v>
@@ -2050,10 +2070,10 @@
         <v>90</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>247</v>
+        <v>228</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="60">
@@ -2061,10 +2081,10 @@
         <v>39</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>133</v>
+        <v>173</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>238</v>
       </c>
       <c r="D28" s="2">
         <v>1887</v>
@@ -2085,13 +2105,13 @@
         <v>90</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" hidden="1">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="15" hidden="1" customHeight="1">
       <c r="A29" s="2">
         <v>40</v>
       </c>
@@ -2119,7 +2139,7 @@
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
     </row>
-    <row r="30" spans="1:11" hidden="1">
+    <row r="30" spans="1:11" ht="15" hidden="1" customHeight="1">
       <c r="A30" s="2">
         <v>40</v>
       </c>
@@ -2147,7 +2167,7 @@
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
     </row>
-    <row r="31" spans="1:11" hidden="1">
+    <row r="31" spans="1:11" ht="15" hidden="1" customHeight="1">
       <c r="A31" s="2">
         <v>40</v>
       </c>
@@ -2155,7 +2175,7 @@
         <v>109</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D31" s="2">
         <v>1986</v>
@@ -2172,7 +2192,7 @@
       <c r="J31" s="2"/>
       <c r="K31" s="2"/>
     </row>
-    <row r="32" spans="1:11" ht="45">
+    <row r="32" spans="1:11" ht="45" customHeight="1">
       <c r="A32" s="2">
         <v>41</v>
       </c>
@@ -2198,13 +2218,13 @@
         <v>90</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" hidden="1">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="15" hidden="1" customHeight="1">
       <c r="A33" s="2">
         <v>42</v>
       </c>
@@ -2236,8 +2256,8 @@
       <c r="B34" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C34" s="2" t="s">
-        <v>133</v>
+      <c r="C34" s="1" t="s">
+        <v>238</v>
       </c>
       <c r="D34" s="2">
         <v>1884</v>
@@ -2258,10 +2278,10 @@
         <v>90</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>248</v>
+        <v>229</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="45">
@@ -2271,8 +2291,8 @@
       <c r="B35" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C35" s="2" t="s">
-        <v>133</v>
+      <c r="C35" s="1" t="s">
+        <v>238</v>
       </c>
       <c r="D35" s="2">
         <v>1923</v>
@@ -2290,13 +2310,13 @@
         <v>90</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" ht="45">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="45" customHeight="1">
       <c r="A36" s="2">
         <v>43</v>
       </c>
@@ -2322,21 +2342,21 @@
         <v>90</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" ht="45">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" ht="45" customHeight="1">
       <c r="A37" s="2">
         <v>43</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="C37" s="2" t="s">
-        <v>127</v>
+      <c r="C37" s="1" t="s">
+        <v>239</v>
       </c>
       <c r="D37" s="2">
         <v>1870</v>
@@ -2357,21 +2377,21 @@
         <v>90</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" ht="30">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" ht="45" customHeight="1">
       <c r="A38" s="2">
         <v>44</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C38" s="2" t="s">
-        <v>127</v>
+      <c r="C38" s="1" t="s">
+        <v>239</v>
       </c>
       <c r="D38" s="2">
         <v>1856</v>
@@ -2392,10 +2412,10 @@
         <v>90</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>249</v>
+        <v>230</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>233</v>
+        <v>214</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="45">
@@ -2405,8 +2425,8 @@
       <c r="B39" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="C39" s="2" t="s">
-        <v>133</v>
+      <c r="C39" s="1" t="s">
+        <v>238</v>
       </c>
       <c r="D39" s="2">
         <v>1900</v>
@@ -2427,10 +2447,10 @@
         <v>90</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>250</v>
+        <v>231</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="45">
@@ -2440,8 +2460,8 @@
       <c r="B40" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C40" s="2" t="s">
-        <v>132</v>
+      <c r="C40" s="1" t="s">
+        <v>240</v>
       </c>
       <c r="D40" s="2">
         <v>1962</v>
@@ -2459,10 +2479,10 @@
         <v>90</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="K40" s="1" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
     <row r="41" spans="1:11" ht="45">
@@ -2472,8 +2492,8 @@
       <c r="B41" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="C41" s="2" t="s">
-        <v>133</v>
+      <c r="C41" s="1" t="s">
+        <v>238</v>
       </c>
       <c r="D41" s="2">
         <v>1902</v>
@@ -2494,10 +2514,10 @@
         <v>90</v>
       </c>
       <c r="J41" s="1" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="K41" s="1" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
     <row r="42" spans="1:11" ht="60">
@@ -2507,8 +2527,8 @@
       <c r="B42" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="C42" s="2" t="s">
-        <v>133</v>
+      <c r="C42" s="1" t="s">
+        <v>238</v>
       </c>
       <c r="D42" s="2">
         <v>1904</v>
@@ -2526,10 +2546,10 @@
         <v>90</v>
       </c>
       <c r="J42" s="1" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="K42" s="1" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
     </row>
     <row r="43" spans="1:11" ht="45">
@@ -2539,8 +2559,8 @@
       <c r="B43" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C43" s="2" t="s">
-        <v>132</v>
+      <c r="C43" s="1" t="s">
+        <v>240</v>
       </c>
       <c r="D43" s="2">
         <v>1939</v>
@@ -2558,13 +2578,13 @@
         <v>90</v>
       </c>
       <c r="J43" s="1" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="K43" s="1" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" ht="45" hidden="1">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" ht="45" customHeight="1">
       <c r="A44" s="2">
         <v>48</v>
       </c>
@@ -2572,7 +2592,7 @@
         <v>93</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D44" s="2">
         <v>1904</v>
@@ -2593,13 +2613,13 @@
         <v>107</v>
       </c>
       <c r="J44" s="1" t="s">
-        <v>213</v>
+        <v>254</v>
       </c>
       <c r="K44" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" ht="30" hidden="1">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" ht="30" customHeight="1">
       <c r="A45" s="2">
         <v>48</v>
       </c>
@@ -2628,13 +2648,13 @@
         <v>107</v>
       </c>
       <c r="J45" s="1" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="K45" s="1" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" ht="45" hidden="1">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" ht="45" customHeight="1">
       <c r="A46" s="2">
         <v>48</v>
       </c>
@@ -2648,7 +2668,7 @@
         <v>1846</v>
       </c>
       <c r="E46" s="2">
-        <v>1881</v>
+        <v>1883</v>
       </c>
       <c r="F46" s="2">
         <v>40.435000000000102</v>
@@ -2663,13 +2683,13 @@
         <v>107</v>
       </c>
       <c r="J46" s="1" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="K46" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" ht="45" hidden="1">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" ht="45" customHeight="1">
       <c r="A47" s="2">
         <v>49</v>
       </c>
@@ -2677,7 +2697,7 @@
         <v>95</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D47" s="2">
         <v>1883</v>
@@ -2695,21 +2715,21 @@
         <v>107</v>
       </c>
       <c r="J47" s="1" t="s">
-        <v>214</v>
+        <v>255</v>
       </c>
       <c r="K47" s="1" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" ht="45" hidden="1">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" ht="45" customHeight="1">
       <c r="A48" s="2">
         <v>53</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D48" s="2">
         <v>1863</v>
@@ -2730,21 +2750,21 @@
         <v>107</v>
       </c>
       <c r="J48" s="1" t="s">
-        <v>215</v>
+        <v>256</v>
       </c>
       <c r="K48" s="1" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" ht="45" hidden="1">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" ht="45" customHeight="1">
       <c r="A49" s="2">
         <v>53</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>253</v>
+        <v>232</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D49" s="2">
         <v>1903</v>
@@ -2762,13 +2782,13 @@
         <v>107</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>216</v>
+        <v>257</v>
       </c>
       <c r="K49" s="1" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11" ht="45" hidden="1">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" ht="45" customHeight="1">
       <c r="A50" s="2">
         <v>54</v>
       </c>
@@ -2776,7 +2796,7 @@
         <v>96</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D50" s="2">
         <v>1928</v>
@@ -2794,13 +2814,13 @@
         <v>107</v>
       </c>
       <c r="J50" s="1" t="s">
-        <v>217</v>
+        <v>258</v>
       </c>
       <c r="K50" s="3" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" ht="30" hidden="1">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" ht="30" customHeight="1">
       <c r="A51" s="2">
         <v>56</v>
       </c>
@@ -2829,13 +2849,13 @@
         <v>107</v>
       </c>
       <c r="J51" s="1" t="s">
-        <v>254</v>
+        <v>259</v>
       </c>
       <c r="K51" s="1" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" ht="45" hidden="1">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" ht="45" customHeight="1">
       <c r="A52" s="2">
         <v>56</v>
       </c>
@@ -2843,7 +2863,7 @@
         <v>98</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D52" s="2">
         <v>1904</v>
@@ -2864,18 +2884,18 @@
         <v>107</v>
       </c>
       <c r="J52" s="1" t="s">
-        <v>218</v>
+        <v>260</v>
       </c>
       <c r="K52" s="1" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" ht="45" hidden="1">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" ht="45" customHeight="1">
       <c r="A53" s="2">
         <v>56</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>255</v>
+        <v>233</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>124</v>
@@ -2896,13 +2916,13 @@
         <v>107</v>
       </c>
       <c r="J53" s="1" t="s">
-        <v>256</v>
+        <v>261</v>
       </c>
       <c r="K53" s="1" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11" ht="45" hidden="1">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" ht="45" customHeight="1">
       <c r="A54" s="2">
         <v>58</v>
       </c>
@@ -2910,7 +2930,7 @@
         <v>99</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D54" s="2">
         <v>1896</v>
@@ -2931,13 +2951,13 @@
         <v>107</v>
       </c>
       <c r="J54" s="1" t="s">
-        <v>219</v>
+        <v>262</v>
       </c>
       <c r="K54" s="1" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11" ht="45" hidden="1">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" ht="45" customHeight="1">
       <c r="A55" s="2">
         <v>59</v>
       </c>
@@ -2963,21 +2983,21 @@
         <v>107</v>
       </c>
       <c r="J55" s="1" t="s">
-        <v>220</v>
+        <v>263</v>
       </c>
       <c r="K55" s="1" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11" ht="30" hidden="1">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" ht="60">
       <c r="A56" s="2">
         <v>60</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>135</v>
+        <v>252</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D56" s="2">
         <v>1887</v>
@@ -2997,19 +3017,22 @@
       <c r="I56" s="2" t="s">
         <v>107</v>
       </c>
+      <c r="J56" s="1" t="s">
+        <v>253</v>
+      </c>
       <c r="K56" s="1" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="57" spans="1:11" ht="30" hidden="1">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" ht="30">
       <c r="A57" s="2">
         <v>60</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>135</v>
+        <v>252</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D57" s="2">
         <v>1901</v>
@@ -3027,33 +3050,30 @@
         <v>107</v>
       </c>
       <c r="J57" s="1" t="s">
-        <v>221</v>
+        <v>246</v>
       </c>
       <c r="K57" s="1" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="58" spans="1:11" ht="45" hidden="1">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" ht="30">
       <c r="A58" s="2">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>101</v>
+        <v>248</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D58" s="2">
-        <v>1895</v>
-      </c>
-      <c r="E58" s="2">
-        <v>1968</v>
+        <v>1904</v>
       </c>
       <c r="F58" s="2">
-        <v>40.3975170000001</v>
+        <v>40.428365999999997</v>
       </c>
       <c r="G58" s="2">
-        <v>-79.935468999999998</v>
+        <v>-79.960593000000003</v>
       </c>
       <c r="H58" s="2" t="s">
         <v>5</v>
@@ -3062,23 +3082,26 @@
         <v>107</v>
       </c>
       <c r="J58" s="1" t="s">
-        <v>222</v>
+        <v>246</v>
       </c>
       <c r="K58" s="1" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="59" spans="1:11" ht="45" hidden="1">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" ht="45" customHeight="1">
       <c r="A59" s="2">
         <v>61</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>257</v>
+        <v>101</v>
       </c>
       <c r="C59" s="2" t="s">
         <v>132</v>
       </c>
       <c r="D59" s="2">
+        <v>1895</v>
+      </c>
+      <c r="E59" s="2">
         <v>1968</v>
       </c>
       <c r="F59" s="2">
@@ -3094,33 +3117,30 @@
         <v>107</v>
       </c>
       <c r="J59" s="1" t="s">
-        <v>223</v>
+        <v>264</v>
       </c>
       <c r="K59" s="1" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="60" spans="1:11" ht="60" hidden="1">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" ht="45" customHeight="1">
       <c r="A60" s="2">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D60" s="2">
-        <v>1884</v>
-      </c>
-      <c r="E60" s="2">
-        <v>1915</v>
+        <v>1968</v>
       </c>
       <c r="F60" s="2">
-        <v>40.398198000000001</v>
+        <v>40.3975170000001</v>
       </c>
       <c r="G60" s="2">
-        <v>-79.931330999999901</v>
+        <v>-79.935468999999998</v>
       </c>
       <c r="H60" s="2" t="s">
         <v>5</v>
@@ -3129,23 +3149,26 @@
         <v>107</v>
       </c>
       <c r="J60" s="1" t="s">
-        <v>258</v>
+        <v>265</v>
       </c>
       <c r="K60" s="1" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="61" spans="1:11" ht="45" hidden="1">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" ht="60" customHeight="1">
       <c r="A61" s="2">
         <v>62</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>236</v>
+        <v>216</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D61" s="2">
+        <v>1884</v>
+      </c>
+      <c r="E61" s="2">
         <v>1915</v>
       </c>
       <c r="F61" s="2">
@@ -3161,33 +3184,30 @@
         <v>107</v>
       </c>
       <c r="J61" s="1" t="s">
-        <v>224</v>
+        <v>266</v>
       </c>
       <c r="K61" s="1" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="62" spans="1:11" ht="45" hidden="1">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" ht="45" customHeight="1">
       <c r="A62" s="2">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>102</v>
+        <v>217</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D62" s="2">
-        <v>1897</v>
-      </c>
-      <c r="E62" s="2">
-        <v>1938</v>
+        <v>1915</v>
       </c>
       <c r="F62" s="2">
-        <v>40.413455000000098</v>
+        <v>40.398198000000001</v>
       </c>
       <c r="G62" s="2">
-        <v>-79.914787000000004</v>
+        <v>-79.931330999999901</v>
       </c>
       <c r="H62" s="2" t="s">
         <v>5</v>
@@ -3196,30 +3216,33 @@
         <v>107</v>
       </c>
       <c r="J62" s="1" t="s">
-        <v>225</v>
+        <v>267</v>
       </c>
       <c r="K62" s="1" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="63" spans="1:11" ht="60" hidden="1">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" ht="45" customHeight="1">
       <c r="A63" s="2">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C63" s="2" t="s">
         <v>132</v>
       </c>
       <c r="D63" s="2">
-        <v>1937</v>
+        <v>1897</v>
+      </c>
+      <c r="E63" s="2">
+        <v>1938</v>
       </c>
       <c r="F63" s="2">
-        <v>40.410668999999999</v>
+        <v>40.413455000000098</v>
       </c>
       <c r="G63" s="2">
-        <v>-79.918432999999894</v>
+        <v>-79.914787000000004</v>
       </c>
       <c r="H63" s="2" t="s">
         <v>5</v>
@@ -3228,65 +3251,62 @@
         <v>107</v>
       </c>
       <c r="J63" s="1" t="s">
-        <v>226</v>
+        <v>268</v>
       </c>
       <c r="K63" s="1" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="64" spans="1:11" ht="45" hidden="1">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" ht="60" customHeight="1">
       <c r="A64" s="2">
+        <v>64</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D64" s="2">
+        <v>1937</v>
+      </c>
+      <c r="F64" s="2">
+        <v>40.410668999999999</v>
+      </c>
+      <c r="G64" s="2">
+        <v>-79.918432999999894</v>
+      </c>
+      <c r="H64" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I64" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="J64" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="K64" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" ht="45" customHeight="1">
+      <c r="A65" s="2">
         <v>66</v>
       </c>
-      <c r="B64" s="1" t="s">
+      <c r="B65" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="C64" s="2" t="s">
+      <c r="C65" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="D64" s="2">
+      <c r="D65" s="2">
         <v>1932</v>
       </c>
-      <c r="F64" s="2">
+      <c r="F65" s="2">
         <v>40.446449999999999</v>
       </c>
-      <c r="G64" s="2">
+      <c r="G65" s="2">
         <v>-80.026889999999995</v>
-      </c>
-      <c r="H64" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="I64" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="J64" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="K64" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="65" spans="1:11" ht="45" hidden="1">
-      <c r="A65" s="2">
-        <v>68</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="C65" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="D65" s="2">
-        <v>1890</v>
-      </c>
-      <c r="E65" s="2">
-        <v>1915</v>
-      </c>
-      <c r="F65" s="2">
-        <v>40.462884000000003</v>
-      </c>
-      <c r="G65" s="2">
-        <v>-80.042850999999999</v>
       </c>
       <c r="H65" s="2" t="s">
         <v>5</v>
@@ -3295,23 +3315,26 @@
         <v>48</v>
       </c>
       <c r="J65" s="1" t="s">
-        <v>229</v>
+        <v>209</v>
       </c>
       <c r="K65" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="66" spans="1:11" ht="45" hidden="1">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" ht="45" customHeight="1">
       <c r="A66" s="2">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>105</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D66" s="2">
+        <v>1890</v>
+      </c>
+      <c r="E66" s="2">
         <v>1915</v>
       </c>
       <c r="F66" s="2">
@@ -3327,30 +3350,30 @@
         <v>48</v>
       </c>
       <c r="J66" s="1" t="s">
-        <v>228</v>
+        <v>211</v>
       </c>
       <c r="K66" s="1" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="67" spans="1:11" ht="45" hidden="1">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" ht="45" customHeight="1">
       <c r="A67" s="2">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="D67" s="2">
-        <v>1931</v>
+        <v>1915</v>
       </c>
       <c r="F67" s="2">
-        <v>40.477150000000101</v>
+        <v>40.462884000000003</v>
       </c>
       <c r="G67" s="2">
-        <v>-80.048500000000004</v>
+        <v>-80.042850999999999</v>
       </c>
       <c r="H67" s="2" t="s">
         <v>5</v>
@@ -3359,52 +3382,60 @@
         <v>48</v>
       </c>
       <c r="J67" s="1" t="s">
-        <v>230</v>
+        <v>210</v>
       </c>
       <c r="K67" s="1" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="68" spans="1:11" hidden="1">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" ht="45" customHeight="1">
       <c r="A68" s="2">
+        <v>71</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D68" s="2">
+        <v>1931</v>
+      </c>
+      <c r="F68" s="2">
+        <v>40.477150000000101</v>
+      </c>
+      <c r="G68" s="2">
+        <v>-80.048500000000004</v>
+      </c>
+      <c r="H68" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I68" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="J68" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="K68" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" ht="15" hidden="1" customHeight="1">
+      <c r="A69" s="2">
         <v>74</v>
       </c>
-      <c r="B68" s="2" t="s">
+      <c r="B69" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="D68" s="2">
+      <c r="C69" s="2"/>
+      <c r="D69" s="2">
         <v>1896</v>
       </c>
-      <c r="F68" s="2">
+      <c r="F69" s="2">
         <v>40.437040000000003</v>
       </c>
-      <c r="G68" s="2">
+      <c r="G69" s="2">
         <v>-79.946728999999905</v>
-      </c>
-      <c r="H68" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J68" s="2"/>
-      <c r="K68" s="2"/>
-    </row>
-    <row r="69" spans="1:11" hidden="1">
-      <c r="A69" s="2">
-        <v>75</v>
-      </c>
-      <c r="B69" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="D69" s="2">
-        <v>1890</v>
-      </c>
-      <c r="E69" s="2">
-        <v>1896</v>
-      </c>
-      <c r="F69" s="2">
-        <v>40.441358000000001</v>
-      </c>
-      <c r="G69" s="2">
-        <v>-79.949285000000003</v>
       </c>
       <c r="H69" s="2" t="s">
         <v>6</v>
@@ -3412,15 +3443,19 @@
       <c r="J69" s="2"/>
       <c r="K69" s="2"/>
     </row>
-    <row r="70" spans="1:11" hidden="1">
+    <row r="70" spans="1:11" ht="15" hidden="1" customHeight="1">
       <c r="A70" s="2">
         <v>75</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>112</v>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="C70" s="2"/>
       <c r="D70" s="2">
-        <v>1897</v>
+        <v>1890</v>
+      </c>
+      <c r="E70" s="2">
+        <v>1896</v>
       </c>
       <c r="F70" s="2">
         <v>40.441358000000001</v>
@@ -3434,21 +3469,22 @@
       <c r="J70" s="2"/>
       <c r="K70" s="2"/>
     </row>
-    <row r="71" spans="1:11" hidden="1">
+    <row r="71" spans="1:11" ht="15" hidden="1" customHeight="1">
       <c r="A71" s="2">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>114</v>
-      </c>
+        <v>112</v>
+      </c>
+      <c r="C71" s="2"/>
       <c r="D71" s="2">
-        <v>1907</v>
+        <v>1897</v>
       </c>
       <c r="F71" s="2">
-        <v>40.434529000000097</v>
+        <v>40.441358000000001</v>
       </c>
       <c r="G71" s="2">
-        <v>-79.950046999999998</v>
+        <v>-79.949285000000003</v>
       </c>
       <c r="H71" s="2" t="s">
         <v>6</v>
@@ -3456,21 +3492,22 @@
       <c r="J71" s="2"/>
       <c r="K71" s="2"/>
     </row>
-    <row r="72" spans="1:11" hidden="1">
+    <row r="72" spans="1:11" ht="15" hidden="1" customHeight="1">
       <c r="A72" s="2">
         <v>76</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>115</v>
-      </c>
+        <v>114</v>
+      </c>
+      <c r="C72" s="2"/>
       <c r="D72" s="2">
-        <v>1940</v>
+        <v>1907</v>
       </c>
       <c r="F72" s="2">
-        <v>40.434404999999998</v>
+        <v>40.434529000000097</v>
       </c>
       <c r="G72" s="2">
-        <v>-79.950137999999995</v>
+        <v>-79.950046999999998</v>
       </c>
       <c r="H72" s="2" t="s">
         <v>6</v>
@@ -3478,24 +3515,22 @@
       <c r="J72" s="2"/>
       <c r="K72" s="2"/>
     </row>
-    <row r="73" spans="1:11" hidden="1">
+    <row r="73" spans="1:11" ht="15" hidden="1" customHeight="1">
       <c r="A73" s="2">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>116</v>
-      </c>
+        <v>115</v>
+      </c>
+      <c r="C73" s="2"/>
       <c r="D73" s="2">
-        <v>1898</v>
-      </c>
-      <c r="E73" s="2">
-        <v>1983</v>
+        <v>1940</v>
       </c>
       <c r="F73" s="2">
-        <v>40.444506146000002</v>
+        <v>40.434404999999998</v>
       </c>
       <c r="G73" s="2">
-        <v>-79.946756172999997</v>
+        <v>-79.950137999999995</v>
       </c>
       <c r="H73" s="2" t="s">
         <v>6</v>
@@ -3503,14 +3538,18 @@
       <c r="J73" s="2"/>
       <c r="K73" s="2"/>
     </row>
-    <row r="74" spans="1:11" hidden="1">
+    <row r="74" spans="1:11" ht="15" hidden="1" customHeight="1">
       <c r="A74" s="2">
         <v>77</v>
       </c>
       <c r="B74" s="2" t="s">
         <v>116</v>
       </c>
+      <c r="C74" s="2"/>
       <c r="D74" s="2">
+        <v>1898</v>
+      </c>
+      <c r="E74" s="2">
         <v>1983</v>
       </c>
       <c r="F74" s="2">
@@ -3525,24 +3564,22 @@
       <c r="J74" s="2"/>
       <c r="K74" s="2"/>
     </row>
-    <row r="75" spans="1:11" hidden="1">
+    <row r="75" spans="1:11" ht="15" hidden="1" customHeight="1">
       <c r="A75" s="2">
         <v>77</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>117</v>
-      </c>
+        <v>116</v>
+      </c>
+      <c r="C75" s="2"/>
       <c r="D75" s="2">
-        <v>1901</v>
-      </c>
-      <c r="E75" s="2">
-        <v>1973</v>
+        <v>1983</v>
       </c>
       <c r="F75" s="2">
-        <v>40.440000000000097</v>
+        <v>40.444506146000002</v>
       </c>
       <c r="G75" s="2">
-        <v>-79.900173999999893</v>
+        <v>-79.946756172999997</v>
       </c>
       <c r="H75" s="2" t="s">
         <v>6</v>
@@ -3550,14 +3587,18 @@
       <c r="J75" s="2"/>
       <c r="K75" s="2"/>
     </row>
-    <row r="76" spans="1:11" hidden="1">
+    <row r="76" spans="1:11" ht="15" hidden="1" customHeight="1">
       <c r="A76" s="2">
         <v>77</v>
       </c>
       <c r="B76" s="2" t="s">
         <v>117</v>
       </c>
+      <c r="C76" s="2"/>
       <c r="D76" s="2">
+        <v>1901</v>
+      </c>
+      <c r="E76" s="2">
         <v>1973</v>
       </c>
       <c r="F76" s="2">
@@ -3572,24 +3613,22 @@
       <c r="J76" s="2"/>
       <c r="K76" s="2"/>
     </row>
-    <row r="77" spans="1:11" hidden="1">
+    <row r="77" spans="1:11" ht="15" hidden="1" customHeight="1">
       <c r="A77" s="2">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>118</v>
-      </c>
+        <v>117</v>
+      </c>
+      <c r="C77" s="2"/>
       <c r="D77" s="2">
-        <v>1883</v>
-      </c>
-      <c r="E77" s="2">
-        <v>1915</v>
+        <v>1973</v>
       </c>
       <c r="F77" s="2">
-        <v>40.427000000000099</v>
+        <v>40.440000000000097</v>
       </c>
       <c r="G77" s="2">
-        <v>-79.950489999999903</v>
+        <v>-79.900173999999893</v>
       </c>
       <c r="H77" s="2" t="s">
         <v>6</v>
@@ -3597,14 +3636,18 @@
       <c r="J77" s="2"/>
       <c r="K77" s="2"/>
     </row>
-    <row r="78" spans="1:11" hidden="1">
+    <row r="78" spans="1:11" ht="15" hidden="1" customHeight="1">
       <c r="A78" s="2">
         <v>78</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>119</v>
-      </c>
+        <v>118</v>
+      </c>
+      <c r="C78" s="2"/>
       <c r="D78" s="2">
+        <v>1883</v>
+      </c>
+      <c r="E78" s="2">
         <v>1915</v>
       </c>
       <c r="F78" s="2">
@@ -3619,21 +3662,22 @@
       <c r="J78" s="2"/>
       <c r="K78" s="2"/>
     </row>
-    <row r="79" spans="1:11" hidden="1">
+    <row r="79" spans="1:11" ht="15" hidden="1" customHeight="1">
       <c r="A79" s="2">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>120</v>
-      </c>
+        <v>119</v>
+      </c>
+      <c r="C79" s="2"/>
       <c r="D79" s="2">
-        <v>1952</v>
+        <v>1915</v>
       </c>
       <c r="F79" s="2">
-        <v>40.427875999999998</v>
+        <v>40.427000000000099</v>
       </c>
       <c r="G79" s="2">
-        <v>-79.949055000000001</v>
+        <v>-79.950489999999903</v>
       </c>
       <c r="H79" s="2" t="s">
         <v>6</v>
@@ -3641,24 +3685,22 @@
       <c r="J79" s="2"/>
       <c r="K79" s="2"/>
     </row>
-    <row r="80" spans="1:11" hidden="1">
+    <row r="80" spans="1:11" ht="15" hidden="1" customHeight="1">
       <c r="A80" s="2">
         <v>79</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>121</v>
-      </c>
+        <v>120</v>
+      </c>
+      <c r="C80" s="2"/>
       <c r="D80" s="2">
-        <v>1880</v>
-      </c>
-      <c r="E80" s="2">
-        <v>1920</v>
+        <v>1952</v>
       </c>
       <c r="F80" s="2">
-        <v>40.435507000000001</v>
+        <v>40.427875999999998</v>
       </c>
       <c r="G80" s="2">
-        <v>-79.957148000000004</v>
+        <v>-79.949055000000001</v>
       </c>
       <c r="H80" s="2" t="s">
         <v>6</v>
@@ -3666,18 +3708,25 @@
       <c r="J80" s="2"/>
       <c r="K80" s="2"/>
     </row>
-    <row r="81" spans="1:11" hidden="1">
+    <row r="81" spans="1:11" ht="15" hidden="1" customHeight="1">
       <c r="A81" s="2">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>9</v>
+        <v>121</v>
+      </c>
+      <c r="C81" s="2"/>
+      <c r="D81" s="2">
+        <v>1880</v>
+      </c>
+      <c r="E81" s="2">
+        <v>1920</v>
       </c>
       <c r="F81" s="2">
-        <v>40.436189000000098</v>
+        <v>40.435507000000001</v>
       </c>
       <c r="G81" s="2">
-        <v>-79.995831999999993</v>
+        <v>-79.957148000000004</v>
       </c>
       <c r="H81" s="2" t="s">
         <v>6</v>
@@ -3685,18 +3734,19 @@
       <c r="J81" s="2"/>
       <c r="K81" s="2"/>
     </row>
-    <row r="82" spans="1:11" hidden="1">
+    <row r="82" spans="1:11" ht="15" hidden="1" customHeight="1">
       <c r="A82" s="2">
         <v>80</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>10</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="C82" s="2"/>
       <c r="F82" s="2">
-        <v>40.436914000000101</v>
+        <v>40.436189000000098</v>
       </c>
       <c r="G82" s="2">
-        <v>-79.972515999999999</v>
+        <v>-79.995831999999993</v>
       </c>
       <c r="H82" s="2" t="s">
         <v>6</v>
@@ -3704,18 +3754,19 @@
       <c r="J82" s="2"/>
       <c r="K82" s="2"/>
     </row>
-    <row r="83" spans="1:11" hidden="1">
+    <row r="83" spans="1:11" ht="15" hidden="1" customHeight="1">
       <c r="A83" s="2">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>8</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="C83" s="2"/>
       <c r="F83" s="2">
-        <v>40.435421000000098</v>
+        <v>40.436914000000101</v>
       </c>
       <c r="G83" s="2">
-        <v>-79.965554999999895</v>
+        <v>-79.972515999999999</v>
       </c>
       <c r="H83" s="2" t="s">
         <v>6</v>
@@ -3723,18 +3774,19 @@
       <c r="J83" s="2"/>
       <c r="K83" s="2"/>
     </row>
-    <row r="84" spans="1:11" hidden="1">
+    <row r="84" spans="1:11" ht="15" hidden="1" customHeight="1">
       <c r="A84" s="2">
         <v>81</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>11</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="C84" s="2"/>
       <c r="F84" s="2">
-        <v>40.435901000000101</v>
+        <v>40.435421000000098</v>
       </c>
       <c r="G84" s="2">
-        <v>-79.965000000000003</v>
+        <v>-79.965554999999895</v>
       </c>
       <c r="H84" s="2" t="s">
         <v>6</v>
@@ -3742,18 +3794,19 @@
       <c r="J84" s="2"/>
       <c r="K84" s="2"/>
     </row>
-    <row r="85" spans="1:11" hidden="1">
+    <row r="85" spans="1:11" ht="15" hidden="1" customHeight="1">
       <c r="A85" s="2">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>12</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="C85" s="2"/>
       <c r="F85" s="2">
-        <v>40.423604000000097</v>
+        <v>40.435901000000101</v>
       </c>
       <c r="G85" s="2">
-        <v>-79.976788999999897</v>
+        <v>-79.965000000000003</v>
       </c>
       <c r="H85" s="2" t="s">
         <v>6</v>
@@ -3761,18 +3814,19 @@
       <c r="J85" s="2"/>
       <c r="K85" s="2"/>
     </row>
-    <row r="86" spans="1:11" hidden="1">
+    <row r="86" spans="1:11" ht="15" hidden="1" customHeight="1">
       <c r="A86" s="2">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>13</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="C86" s="2"/>
       <c r="F86" s="2">
-        <v>40.423226000000099</v>
+        <v>40.423604000000097</v>
       </c>
       <c r="G86" s="2">
-        <v>-79.974397999999994</v>
+        <v>-79.976788999999897</v>
       </c>
       <c r="H86" s="2" t="s">
         <v>6</v>
@@ -3780,18 +3834,19 @@
       <c r="J86" s="2"/>
       <c r="K86" s="2"/>
     </row>
-    <row r="87" spans="1:11" hidden="1">
+    <row r="87" spans="1:11" ht="15" hidden="1" customHeight="1">
       <c r="A87" s="2">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>16</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="C87" s="2"/>
       <c r="F87" s="2">
-        <v>40.456966000000101</v>
+        <v>40.423226000000099</v>
       </c>
       <c r="G87" s="2">
-        <v>-79.947509999999994</v>
+        <v>-79.974397999999994</v>
       </c>
       <c r="H87" s="2" t="s">
         <v>6</v>
@@ -3799,18 +3854,19 @@
       <c r="J87" s="2"/>
       <c r="K87" s="2"/>
     </row>
-    <row r="88" spans="1:11" hidden="1">
+    <row r="88" spans="1:11" ht="15" hidden="1" customHeight="1">
       <c r="A88" s="2">
         <v>84</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>17</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="C88" s="2"/>
       <c r="F88" s="2">
-        <v>40.426149000000102</v>
+        <v>40.456966000000101</v>
       </c>
       <c r="G88" s="2">
-        <v>-79.937781999999999</v>
+        <v>-79.947509999999994</v>
       </c>
       <c r="H88" s="2" t="s">
         <v>6</v>
@@ -3818,18 +3874,19 @@
       <c r="J88" s="2"/>
       <c r="K88" s="2"/>
     </row>
-    <row r="89" spans="1:11" hidden="1">
+    <row r="89" spans="1:11" ht="15" hidden="1" customHeight="1">
       <c r="A89" s="2">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>15</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="C89" s="2"/>
       <c r="F89" s="2">
-        <v>40.453866000000097</v>
+        <v>40.426149000000102</v>
       </c>
       <c r="G89" s="2">
-        <v>-79.937380000000005</v>
+        <v>-79.937781999999999</v>
       </c>
       <c r="H89" s="2" t="s">
         <v>6</v>
@@ -3837,18 +3894,19 @@
       <c r="J89" s="2"/>
       <c r="K89" s="2"/>
     </row>
-    <row r="90" spans="1:11" hidden="1">
+    <row r="90" spans="1:11" ht="15" hidden="1" customHeight="1">
       <c r="A90" s="2">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>14</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="C90" s="2"/>
       <c r="F90" s="2">
-        <v>40.4608050000001</v>
+        <v>40.453866000000097</v>
       </c>
       <c r="G90" s="2">
-        <v>-79.955464999999904</v>
+        <v>-79.937380000000005</v>
       </c>
       <c r="H90" s="2" t="s">
         <v>6</v>
@@ -3856,18 +3914,19 @@
       <c r="J90" s="2"/>
       <c r="K90" s="2"/>
     </row>
-    <row r="91" spans="1:11" hidden="1">
+    <row r="91" spans="1:11" ht="15" hidden="1" customHeight="1">
       <c r="A91" s="2">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>21</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="C91" s="2"/>
       <c r="F91" s="2">
-        <v>40.472322000000098</v>
+        <v>40.4608050000001</v>
       </c>
       <c r="G91" s="2">
-        <v>-80.004901000000004</v>
+        <v>-79.955464999999904</v>
       </c>
       <c r="H91" s="2" t="s">
         <v>6</v>
@@ -3875,18 +3934,19 @@
       <c r="J91" s="2"/>
       <c r="K91" s="2"/>
     </row>
-    <row r="92" spans="1:11" hidden="1">
+    <row r="92" spans="1:11" ht="15" hidden="1" customHeight="1">
       <c r="A92" s="2">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>18</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="C92" s="2"/>
       <c r="F92" s="2">
-        <v>40.471502999999998</v>
+        <v>40.472322000000098</v>
       </c>
       <c r="G92" s="2">
-        <v>-80.036794</v>
+        <v>-80.004901000000004</v>
       </c>
       <c r="H92" s="2" t="s">
         <v>6</v>
@@ -3894,18 +3954,19 @@
       <c r="J92" s="2"/>
       <c r="K92" s="2"/>
     </row>
-    <row r="93" spans="1:11" hidden="1">
+    <row r="93" spans="1:11" ht="15" hidden="1" customHeight="1">
       <c r="A93" s="2">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>19</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="C93" s="2"/>
       <c r="F93" s="2">
-        <v>40.4760840000001</v>
+        <v>40.471502999999998</v>
       </c>
       <c r="G93" s="2">
-        <v>-80.032714999999897</v>
+        <v>-80.036794</v>
       </c>
       <c r="H93" s="2" t="s">
         <v>6</v>
@@ -3913,18 +3974,19 @@
       <c r="J93" s="2"/>
       <c r="K93" s="2"/>
     </row>
-    <row r="94" spans="1:11" hidden="1">
+    <row r="94" spans="1:11" ht="15" hidden="1" customHeight="1">
       <c r="A94" s="2">
         <v>90</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>20</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="C94" s="2"/>
       <c r="F94" s="2">
-        <v>40.481794999999998</v>
+        <v>40.4760840000001</v>
       </c>
       <c r="G94" s="2">
-        <v>-80.025806000000003</v>
+        <v>-80.032714999999897</v>
       </c>
       <c r="H94" s="2" t="s">
         <v>6</v>
@@ -3932,18 +3994,19 @@
       <c r="J94" s="2"/>
       <c r="K94" s="2"/>
     </row>
-    <row r="95" spans="1:11" hidden="1">
+    <row r="95" spans="1:11" ht="15" hidden="1" customHeight="1">
       <c r="A95" s="2">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>22</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="C95" s="2"/>
       <c r="F95" s="2">
-        <v>40.441986999999997</v>
+        <v>40.481794999999998</v>
       </c>
       <c r="G95" s="2">
-        <v>-79.951903000000001</v>
+        <v>-80.025806000000003</v>
       </c>
       <c r="H95" s="2" t="s">
         <v>6</v>
@@ -3951,18 +4014,19 @@
       <c r="J95" s="2"/>
       <c r="K95" s="2"/>
     </row>
-    <row r="96" spans="1:11" hidden="1">
+    <row r="96" spans="1:11" ht="15" hidden="1" customHeight="1">
       <c r="A96" s="2">
         <v>92</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>23</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="C96" s="2"/>
       <c r="F96" s="2">
-        <v>40.434003000000097</v>
+        <v>40.441986999999997</v>
       </c>
       <c r="G96" s="2">
-        <v>-79.935597999999999</v>
+        <v>-79.951903000000001</v>
       </c>
       <c r="H96" s="2" t="s">
         <v>6</v>
@@ -3970,18 +4034,19 @@
       <c r="J96" s="2"/>
       <c r="K96" s="2"/>
     </row>
-    <row r="97" spans="1:11" hidden="1">
+    <row r="97" spans="1:11" ht="15" hidden="1" customHeight="1">
       <c r="A97" s="2">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>24</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="C97" s="2"/>
       <c r="F97" s="2">
-        <v>40.462701000000003</v>
+        <v>40.434003000000097</v>
       </c>
       <c r="G97" s="2">
-        <v>-79.905410000000003</v>
+        <v>-79.935597999999999</v>
       </c>
       <c r="H97" s="2" t="s">
         <v>6</v>
@@ -3989,18 +4054,19 @@
       <c r="J97" s="2"/>
       <c r="K97" s="2"/>
     </row>
-    <row r="98" spans="1:11" hidden="1">
+    <row r="98" spans="1:11" ht="15" hidden="1" customHeight="1">
       <c r="A98" s="2">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>25</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="C98" s="2"/>
       <c r="F98" s="2">
-        <v>40.466919000000097</v>
+        <v>40.462701000000003</v>
       </c>
       <c r="G98" s="2">
-        <v>-79.915979999999905</v>
+        <v>-79.905410000000003</v>
       </c>
       <c r="H98" s="2" t="s">
         <v>6</v>
@@ -4008,18 +4074,19 @@
       <c r="J98" s="2"/>
       <c r="K98" s="2"/>
     </row>
-    <row r="99" spans="1:11" hidden="1">
+    <row r="99" spans="1:11" ht="15" hidden="1" customHeight="1">
       <c r="A99" s="2">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>26</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="C99" s="2"/>
       <c r="F99" s="2">
-        <v>40.467417000000097</v>
+        <v>40.466919000000097</v>
       </c>
       <c r="G99" s="2">
-        <v>-79.908690000000007</v>
+        <v>-79.915979999999905</v>
       </c>
       <c r="H99" s="2" t="s">
         <v>6</v>
@@ -4027,18 +4094,19 @@
       <c r="J99" s="2"/>
       <c r="K99" s="2"/>
     </row>
-    <row r="100" spans="1:11" hidden="1">
+    <row r="100" spans="1:11" ht="15" hidden="1" customHeight="1">
       <c r="A100" s="2">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>27</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="C100" s="2"/>
       <c r="F100" s="2">
-        <v>40.464685000000003</v>
+        <v>40.467417000000097</v>
       </c>
       <c r="G100" s="2">
-        <v>-79.918912000000006</v>
+        <v>-79.908690000000007</v>
       </c>
       <c r="H100" s="2" t="s">
         <v>6</v>
@@ -4046,18 +4114,19 @@
       <c r="J100" s="2"/>
       <c r="K100" s="2"/>
     </row>
-    <row r="101" spans="1:11" hidden="1">
+    <row r="101" spans="1:11" ht="15" hidden="1" customHeight="1">
       <c r="A101" s="2">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>28</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="C101" s="2"/>
       <c r="F101" s="2">
-        <v>40.455281000000099</v>
+        <v>40.464685000000003</v>
       </c>
       <c r="G101" s="2">
-        <v>-79.944192999999999</v>
+        <v>-79.918912000000006</v>
       </c>
       <c r="H101" s="2" t="s">
         <v>6</v>
@@ -4065,18 +4134,19 @@
       <c r="J101" s="2"/>
       <c r="K101" s="2"/>
     </row>
-    <row r="102" spans="1:11" hidden="1">
+    <row r="102" spans="1:11" ht="15" hidden="1" customHeight="1">
       <c r="A102" s="2">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>29</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="C102" s="2"/>
       <c r="F102" s="2">
-        <v>40.454044000000103</v>
+        <v>40.455281000000099</v>
       </c>
       <c r="G102" s="2">
-        <v>-79.950176999999897</v>
+        <v>-79.944192999999999</v>
       </c>
       <c r="H102" s="2" t="s">
         <v>6</v>
@@ -4084,18 +4154,19 @@
       <c r="J102" s="2"/>
       <c r="K102" s="2"/>
     </row>
-    <row r="103" spans="1:11" hidden="1">
+    <row r="103" spans="1:11" ht="15" hidden="1" customHeight="1">
       <c r="A103" s="2">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>30</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="C103" s="2"/>
       <c r="F103" s="2">
-        <v>40.426760000000101</v>
+        <v>40.454044000000103</v>
       </c>
       <c r="G103" s="2">
-        <v>-79.927091000000004</v>
+        <v>-79.950176999999897</v>
       </c>
       <c r="H103" s="2" t="s">
         <v>6</v>
@@ -4103,18 +4174,19 @@
       <c r="J103" s="2"/>
       <c r="K103" s="2"/>
     </row>
-    <row r="104" spans="1:11" hidden="1">
+    <row r="104" spans="1:11" ht="15" hidden="1" customHeight="1">
       <c r="A104" s="2">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>31</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="C104" s="2"/>
       <c r="F104" s="2">
-        <v>40.487585000000003</v>
+        <v>40.426760000000101</v>
       </c>
       <c r="G104" s="2">
-        <v>-79.919021000000001</v>
+        <v>-79.927091000000004</v>
       </c>
       <c r="H104" s="2" t="s">
         <v>6</v>
@@ -4122,18 +4194,19 @@
       <c r="J104" s="2"/>
       <c r="K104" s="2"/>
     </row>
-    <row r="105" spans="1:11" hidden="1">
+    <row r="105" spans="1:11" ht="15" hidden="1" customHeight="1">
       <c r="A105" s="2">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>32</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="C105" s="2"/>
       <c r="F105" s="2">
-        <v>40.428625000000103</v>
+        <v>40.487585000000003</v>
       </c>
       <c r="G105" s="2">
-        <v>-79.937871999999999</v>
+        <v>-79.919021000000001</v>
       </c>
       <c r="H105" s="2" t="s">
         <v>6</v>
@@ -4141,18 +4214,19 @@
       <c r="J105" s="2"/>
       <c r="K105" s="2"/>
     </row>
-    <row r="106" spans="1:11" hidden="1">
+    <row r="106" spans="1:11" ht="15" hidden="1" customHeight="1">
       <c r="A106" s="2">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>33</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="C106" s="2"/>
       <c r="F106" s="2">
-        <v>40.430383000000099</v>
+        <v>40.428625000000103</v>
       </c>
       <c r="G106" s="2">
-        <v>-80.002347999999998</v>
+        <v>-79.937871999999999</v>
       </c>
       <c r="H106" s="2" t="s">
         <v>6</v>
@@ -4160,18 +4234,19 @@
       <c r="J106" s="2"/>
       <c r="K106" s="2"/>
     </row>
-    <row r="107" spans="1:11" hidden="1">
+    <row r="107" spans="1:11" ht="15" hidden="1" customHeight="1">
       <c r="A107" s="2">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>34</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="C107" s="2"/>
       <c r="F107" s="2">
-        <v>40.4879770000001</v>
+        <v>40.430383000000099</v>
       </c>
       <c r="G107" s="2">
-        <v>-80.045779999999993</v>
+        <v>-80.002347999999998</v>
       </c>
       <c r="H107" s="2" t="s">
         <v>6</v>
@@ -4179,18 +4254,19 @@
       <c r="J107" s="2"/>
       <c r="K107" s="2"/>
     </row>
-    <row r="108" spans="1:11" hidden="1">
+    <row r="108" spans="1:11" ht="15" hidden="1" customHeight="1">
       <c r="A108" s="2">
         <v>108</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>35</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="C108" s="2"/>
       <c r="F108" s="2">
-        <v>40.413918000000102</v>
+        <v>40.4879770000001</v>
       </c>
       <c r="G108" s="2">
-        <v>-79.995039000000006</v>
+        <v>-80.045779999999993</v>
       </c>
       <c r="H108" s="2" t="s">
         <v>6</v>
@@ -4198,18 +4274,19 @@
       <c r="J108" s="2"/>
       <c r="K108" s="2"/>
     </row>
-    <row r="109" spans="1:11" hidden="1">
+    <row r="109" spans="1:11" ht="15" hidden="1" customHeight="1">
       <c r="A109" s="2">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>36</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="C109" s="2"/>
       <c r="F109" s="2">
-        <v>40.4715810000001</v>
+        <v>40.413918000000102</v>
       </c>
       <c r="G109" s="2">
-        <v>-80.037585000000007</v>
+        <v>-79.995039000000006</v>
       </c>
       <c r="H109" s="2" t="s">
         <v>6</v>
@@ -4217,18 +4294,19 @@
       <c r="J109" s="2"/>
       <c r="K109" s="2"/>
     </row>
-    <row r="110" spans="1:11" hidden="1">
+    <row r="110" spans="1:11" ht="15" hidden="1" customHeight="1">
       <c r="A110" s="2">
         <v>109</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>37</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="C110" s="2"/>
       <c r="F110" s="2">
-        <v>40.479965</v>
+        <v>40.4715810000001</v>
       </c>
       <c r="G110" s="2">
-        <v>-80.044217999999901</v>
+        <v>-80.037585000000007</v>
       </c>
       <c r="H110" s="2" t="s">
         <v>6</v>
@@ -4236,18 +4314,19 @@
       <c r="J110" s="2"/>
       <c r="K110" s="2"/>
     </row>
-    <row r="111" spans="1:11" hidden="1">
+    <row r="111" spans="1:11" ht="15" hidden="1" customHeight="1">
       <c r="A111" s="2">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>38</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="C111" s="2"/>
       <c r="F111" s="2">
-        <v>40.484208000000102</v>
+        <v>40.479965</v>
       </c>
       <c r="G111" s="2">
-        <v>-80.050618</v>
+        <v>-80.044217999999901</v>
       </c>
       <c r="H111" s="2" t="s">
         <v>6</v>
@@ -4255,18 +4334,19 @@
       <c r="J111" s="2"/>
       <c r="K111" s="2"/>
     </row>
-    <row r="112" spans="1:11" hidden="1">
+    <row r="112" spans="1:11" ht="15" hidden="1" customHeight="1">
       <c r="A112" s="2">
         <v>110</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>39</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="C112" s="2"/>
       <c r="F112" s="2">
-        <v>40.425566000000103</v>
+        <v>40.484208000000102</v>
       </c>
       <c r="G112" s="2">
-        <v>-79.906165000000001</v>
+        <v>-80.050618</v>
       </c>
       <c r="H112" s="2" t="s">
         <v>6</v>
@@ -4274,18 +4354,19 @@
       <c r="J112" s="2"/>
       <c r="K112" s="2"/>
     </row>
-    <row r="113" spans="1:11" hidden="1">
+    <row r="113" spans="1:11" ht="15" hidden="1" customHeight="1">
       <c r="A113" s="2">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>40</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="C113" s="2"/>
       <c r="F113" s="2">
-        <v>40.458688000000102</v>
+        <v>40.425566000000103</v>
       </c>
       <c r="G113" s="2">
-        <v>-79.926560999999893</v>
+        <v>-79.906165000000001</v>
       </c>
       <c r="H113" s="2" t="s">
         <v>6</v>
@@ -4293,18 +4374,19 @@
       <c r="J113" s="2"/>
       <c r="K113" s="2"/>
     </row>
-    <row r="114" spans="1:11" hidden="1">
+    <row r="114" spans="1:11" ht="15" hidden="1" customHeight="1">
       <c r="A114" s="2">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>41</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="C114" s="2"/>
       <c r="F114" s="2">
-        <v>40.459000000000103</v>
+        <v>40.458688000000102</v>
       </c>
       <c r="G114" s="2">
-        <v>-79.9251</v>
+        <v>-79.926560999999893</v>
       </c>
       <c r="H114" s="2" t="s">
         <v>6</v>
@@ -4312,18 +4394,19 @@
       <c r="J114" s="2"/>
       <c r="K114" s="2"/>
     </row>
-    <row r="115" spans="1:11" hidden="1">
+    <row r="115" spans="1:11" ht="15" hidden="1" customHeight="1">
       <c r="A115" s="2">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>42</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="C115" s="2"/>
       <c r="F115" s="2">
-        <v>40.456245000000102</v>
+        <v>40.459000000000103</v>
       </c>
       <c r="G115" s="2">
-        <v>-79.926766000000001</v>
+        <v>-79.9251</v>
       </c>
       <c r="H115" s="2" t="s">
         <v>6</v>
@@ -4331,18 +4414,19 @@
       <c r="J115" s="2"/>
       <c r="K115" s="2"/>
     </row>
-    <row r="116" spans="1:11" hidden="1">
+    <row r="116" spans="1:11" ht="15" hidden="1" customHeight="1">
       <c r="A116" s="2">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>43</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="C116" s="2"/>
       <c r="F116" s="2">
-        <v>40.454606000000098</v>
+        <v>40.456245000000102</v>
       </c>
       <c r="G116" s="2">
-        <v>-79.942988999999997</v>
+        <v>-79.926766000000001</v>
       </c>
       <c r="H116" s="2" t="s">
         <v>6</v>
@@ -4350,18 +4434,19 @@
       <c r="J116" s="2"/>
       <c r="K116" s="2"/>
     </row>
-    <row r="117" spans="1:11" hidden="1">
+    <row r="117" spans="1:11" ht="15" hidden="1" customHeight="1">
       <c r="A117" s="2">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>44</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="C117" s="2"/>
       <c r="F117" s="2">
-        <v>40.459586000000101</v>
+        <v>40.454606000000098</v>
       </c>
       <c r="G117" s="2">
-        <v>-79.966154000000003</v>
+        <v>-79.942988999999997</v>
       </c>
       <c r="H117" s="2" t="s">
         <v>6</v>
@@ -4369,18 +4454,19 @@
       <c r="J117" s="2"/>
       <c r="K117" s="2"/>
     </row>
-    <row r="118" spans="1:11" hidden="1">
+    <row r="118" spans="1:11" ht="15" hidden="1" customHeight="1">
       <c r="A118" s="2">
         <v>116</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>45</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="C118" s="2"/>
       <c r="F118" s="2">
-        <v>40.4559</v>
+        <v>40.459586000000101</v>
       </c>
       <c r="G118" s="2">
-        <v>-79.973299999999895</v>
+        <v>-79.966154000000003</v>
       </c>
       <c r="H118" s="2" t="s">
         <v>6</v>
@@ -4388,18 +4474,19 @@
       <c r="J118" s="2"/>
       <c r="K118" s="2"/>
     </row>
-    <row r="119" spans="1:11" hidden="1">
+    <row r="119" spans="1:11" ht="15" hidden="1" customHeight="1">
       <c r="A119" s="2">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>46</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="C119" s="2"/>
       <c r="F119" s="2">
-        <v>40.406973999999998</v>
+        <v>40.4559</v>
       </c>
       <c r="G119" s="2">
-        <v>-79.944084000000004</v>
+        <v>-79.973299999999895</v>
       </c>
       <c r="H119" s="2" t="s">
         <v>6</v>
@@ -4407,18 +4494,19 @@
       <c r="J119" s="2"/>
       <c r="K119" s="2"/>
     </row>
-    <row r="120" spans="1:11" hidden="1">
+    <row r="120" spans="1:11" ht="15" hidden="1" customHeight="1">
       <c r="A120" s="2">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>47</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="C120" s="2"/>
       <c r="F120" s="2">
-        <v>40.427770000000102</v>
+        <v>40.406973999999998</v>
       </c>
       <c r="G120" s="2">
-        <v>-79.992890000000003</v>
+        <v>-79.944084000000004</v>
       </c>
       <c r="H120" s="2" t="s">
         <v>6</v>
@@ -4426,18 +4514,19 @@
       <c r="J120" s="2"/>
       <c r="K120" s="2"/>
     </row>
-    <row r="121" spans="1:11" hidden="1">
+    <row r="121" spans="1:11" ht="15" hidden="1" customHeight="1">
       <c r="A121" s="2">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>48</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="C121" s="2"/>
       <c r="F121" s="2">
-        <v>40.451634000000098</v>
+        <v>40.427770000000102</v>
       </c>
       <c r="G121" s="2">
-        <v>-80.010687000000004</v>
+        <v>-79.992890000000003</v>
       </c>
       <c r="H121" s="2" t="s">
         <v>6</v>
@@ -4445,18 +4534,19 @@
       <c r="J121" s="2"/>
       <c r="K121" s="2"/>
     </row>
-    <row r="122" spans="1:11" hidden="1">
+    <row r="122" spans="1:11" ht="15" hidden="1" customHeight="1">
       <c r="A122" s="2">
         <v>120</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>49</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="C122" s="2"/>
       <c r="F122" s="2">
-        <v>40.4539520000001</v>
+        <v>40.451634000000098</v>
       </c>
       <c r="G122" s="2">
-        <v>-80.014623999999998</v>
+        <v>-80.010687000000004</v>
       </c>
       <c r="H122" s="2" t="s">
         <v>6</v>
@@ -4464,18 +4554,19 @@
       <c r="J122" s="2"/>
       <c r="K122" s="2"/>
     </row>
-    <row r="123" spans="1:11" hidden="1">
+    <row r="123" spans="1:11" ht="15" hidden="1" customHeight="1">
       <c r="A123" s="2">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>50</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="C123" s="2"/>
       <c r="F123" s="2">
-        <v>40.458554999999997</v>
+        <v>40.4539520000001</v>
       </c>
       <c r="G123" s="2">
-        <v>-80.023665999999906</v>
+        <v>-80.014623999999998</v>
       </c>
       <c r="H123" s="2" t="s">
         <v>6</v>
@@ -4483,18 +4574,19 @@
       <c r="J123" s="2"/>
       <c r="K123" s="2"/>
     </row>
-    <row r="124" spans="1:11" hidden="1">
+    <row r="124" spans="1:11" ht="15" hidden="1" customHeight="1">
       <c r="A124" s="2">
         <v>121</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>51</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="C124" s="2"/>
       <c r="F124" s="2">
-        <v>40.461849000000001</v>
+        <v>40.458554999999997</v>
       </c>
       <c r="G124" s="2">
-        <v>-80.031160999999898</v>
+        <v>-80.023665999999906</v>
       </c>
       <c r="H124" s="2" t="s">
         <v>6</v>
@@ -4502,18 +4594,19 @@
       <c r="J124" s="2"/>
       <c r="K124" s="2"/>
     </row>
-    <row r="125" spans="1:11" hidden="1">
+    <row r="125" spans="1:11" ht="15" hidden="1" customHeight="1">
       <c r="A125" s="2">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>52</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="C125" s="2"/>
       <c r="F125" s="2">
-        <v>40.452952000000003</v>
+        <v>40.461849000000001</v>
       </c>
       <c r="G125" s="2">
-        <v>-80.054523000000003</v>
+        <v>-80.031160999999898</v>
       </c>
       <c r="H125" s="2" t="s">
         <v>6</v>
@@ -4521,18 +4614,19 @@
       <c r="J125" s="2"/>
       <c r="K125" s="2"/>
     </row>
-    <row r="126" spans="1:11" hidden="1">
+    <row r="126" spans="1:11" ht="15" hidden="1" customHeight="1">
       <c r="A126" s="2">
         <v>122</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>53</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="C126" s="2"/>
       <c r="F126" s="2">
-        <v>40.433608999999997</v>
+        <v>40.452952000000003</v>
       </c>
       <c r="G126" s="2">
-        <v>-80.034202999999906</v>
+        <v>-80.054523000000003</v>
       </c>
       <c r="H126" s="2" t="s">
         <v>6</v>
@@ -4540,18 +4634,19 @@
       <c r="J126" s="2"/>
       <c r="K126" s="2"/>
     </row>
-    <row r="127" spans="1:11" hidden="1">
+    <row r="127" spans="1:11" ht="15" hidden="1" customHeight="1">
       <c r="A127" s="2">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>54</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="C127" s="2"/>
       <c r="F127" s="2">
-        <v>40.415566000000098</v>
+        <v>40.433608999999997</v>
       </c>
       <c r="G127" s="2">
-        <v>-79.916652999999897</v>
+        <v>-80.034202999999906</v>
       </c>
       <c r="H127" s="2" t="s">
         <v>6</v>
@@ -4559,18 +4654,19 @@
       <c r="J127" s="2"/>
       <c r="K127" s="2"/>
     </row>
-    <row r="128" spans="1:11" hidden="1">
+    <row r="128" spans="1:11" ht="15" hidden="1" customHeight="1">
       <c r="A128" s="2">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>55</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="C128" s="2"/>
       <c r="F128" s="2">
-        <v>40.418851000000103</v>
+        <v>40.415566000000098</v>
       </c>
       <c r="G128" s="2">
-        <v>-79.948326999999907</v>
+        <v>-79.916652999999897</v>
       </c>
       <c r="H128" s="2" t="s">
         <v>6</v>
@@ -4578,18 +4674,19 @@
       <c r="J128" s="2"/>
       <c r="K128" s="2"/>
     </row>
-    <row r="129" spans="1:11" hidden="1">
+    <row r="129" spans="1:11" ht="15" hidden="1" customHeight="1">
       <c r="A129" s="2">
         <v>125</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>56</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="C129" s="2"/>
       <c r="F129" s="2">
-        <v>40.443394000000097</v>
+        <v>40.418851000000103</v>
       </c>
       <c r="G129" s="2">
-        <v>-79.992804000000007</v>
+        <v>-79.948326999999907</v>
       </c>
       <c r="H129" s="2" t="s">
         <v>6</v>
@@ -4597,18 +4694,19 @@
       <c r="J129" s="2"/>
       <c r="K129" s="2"/>
     </row>
-    <row r="130" spans="1:11" hidden="1">
+    <row r="130" spans="1:11" ht="15" hidden="1" customHeight="1">
       <c r="A130" s="2">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>57</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="C130" s="2"/>
       <c r="F130" s="2">
-        <v>40.457135999999998</v>
+        <v>40.443394000000097</v>
       </c>
       <c r="G130" s="2">
-        <v>-79.988479999999996</v>
+        <v>-79.992804000000007</v>
       </c>
       <c r="H130" s="2" t="s">
         <v>6</v>
@@ -4616,18 +4714,19 @@
       <c r="J130" s="2"/>
       <c r="K130" s="2"/>
     </row>
-    <row r="131" spans="1:11" hidden="1">
+    <row r="131" spans="1:11" ht="15" hidden="1" customHeight="1">
       <c r="A131" s="2">
         <v>126</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>58</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="C131" s="2"/>
       <c r="F131" s="2">
-        <v>40.485859000000097</v>
+        <v>40.457135999999998</v>
       </c>
       <c r="G131" s="2">
-        <v>-80.045368999999894</v>
+        <v>-79.988479999999996</v>
       </c>
       <c r="H131" s="2" t="s">
         <v>6</v>
@@ -4635,18 +4734,19 @@
       <c r="J131" s="2"/>
       <c r="K131" s="2"/>
     </row>
-    <row r="132" spans="1:11" hidden="1">
+    <row r="132" spans="1:11" ht="15" hidden="1" customHeight="1">
       <c r="A132" s="2">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>59</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="C132" s="2"/>
       <c r="F132" s="2">
-        <v>40.461343000000099</v>
+        <v>40.485859000000097</v>
       </c>
       <c r="G132" s="2">
-        <v>-80.053490999999994</v>
+        <v>-80.045368999999894</v>
       </c>
       <c r="H132" s="2" t="s">
         <v>6</v>
@@ -4654,18 +4754,19 @@
       <c r="J132" s="2"/>
       <c r="K132" s="2"/>
     </row>
-    <row r="133" spans="1:11" hidden="1">
+    <row r="133" spans="1:11" ht="15" hidden="1" customHeight="1">
       <c r="A133" s="2">
         <v>127</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>60</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="C133" s="2"/>
       <c r="F133" s="2">
-        <v>40.463341000000099</v>
+        <v>40.461343000000099</v>
       </c>
       <c r="G133" s="2">
-        <v>-80.074088000000003</v>
+        <v>-80.053490999999994</v>
       </c>
       <c r="H133" s="2" t="s">
         <v>6</v>
@@ -4673,19 +4774,35 @@
       <c r="J133" s="2"/>
       <c r="K133" s="2"/>
     </row>
+    <row r="134" spans="1:11" ht="15" hidden="1" customHeight="1">
+      <c r="A134" s="2">
+        <v>127</v>
+      </c>
+      <c r="B134" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C134" s="2"/>
+      <c r="F134" s="2">
+        <v>40.463341000000099</v>
+      </c>
+      <c r="G134" s="2">
+        <v>-80.074088000000003</v>
+      </c>
+      <c r="H134" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J134" s="2"/>
+      <c r="K134" s="2"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:K133">
+  <autoFilter ref="A1:K134">
     <filterColumn colId="2"/>
     <filterColumn colId="7">
       <filters>
         <filter val="Y"/>
       </filters>
     </filterColumn>
-    <filterColumn colId="8">
-      <filters>
-        <filter val="Allegheny"/>
-      </filters>
-    </filterColumn>
+    <filterColumn colId="8"/>
     <filterColumn colId="9"/>
     <sortState ref="A2:K132">
       <sortCondition ref="A1:A132"/>

</xml_diff>